<commit_message>
update passed_time generation logic
</commit_message>
<xml_diff>
--- a/漏洞跟踪表_模板数据.xlsx
+++ b/漏洞跟踪表_模板数据.xlsx
@@ -580,7 +580,7 @@
       </c>
       <c r="H2" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I2" s="7" t="inlineStr"/>
@@ -631,7 +631,7 @@
       </c>
       <c r="H3" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I3" s="7" t="inlineStr"/>
@@ -733,7 +733,7 @@
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr"/>
@@ -784,7 +784,7 @@
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I7" s="7" t="inlineStr"/>
@@ -886,7 +886,7 @@
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I8" s="7" t="inlineStr"/>
@@ -937,7 +937,7 @@
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I9" s="7" t="inlineStr"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I10" s="7" t="inlineStr"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr"/>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="H12" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I12" s="7" t="inlineStr"/>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I13" s="7" t="inlineStr"/>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I15" s="7" t="inlineStr"/>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="H16" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I16" s="7" t="inlineStr"/>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H17" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I17" s="7" t="inlineStr"/>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="H18" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I18" s="7" t="inlineStr"/>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="H19" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I19" s="7" t="inlineStr"/>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="H20" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I20" s="7" t="inlineStr"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="H21" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I21" s="7" t="inlineStr"/>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="H22" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I22" s="7" t="inlineStr"/>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="H23" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I23" s="7" t="inlineStr"/>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="H24" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I24" s="7" t="inlineStr"/>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="H25" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I25" s="7" t="inlineStr"/>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="H27" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I27" s="7" t="inlineStr"/>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="H28" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I28" s="7" t="inlineStr"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="H29" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I29" s="7" t="inlineStr"/>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="H30" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I30" s="7" t="inlineStr"/>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="H31" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I31" s="7" t="inlineStr"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="H32" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I32" s="7" t="inlineStr"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="H34" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I34" s="7" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="H35" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I35" s="7" t="inlineStr"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="H36" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I36" s="7" t="inlineStr"/>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="H37" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I37" s="7" t="inlineStr"/>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="H38" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I38" s="7" t="inlineStr"/>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="H39" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I39" s="7" t="inlineStr"/>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="H40" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I40" s="7" t="inlineStr"/>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="H41" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I41" s="7" t="inlineStr"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="H42" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I42" s="7" t="inlineStr"/>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="H43" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I43" s="7" t="inlineStr"/>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="H44" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I44" s="7" t="inlineStr"/>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="H46" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I46" s="7" t="inlineStr"/>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="H47" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I47" s="7" t="inlineStr"/>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="H48" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I48" s="7" t="inlineStr"/>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H49" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I49" s="7" t="inlineStr"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="H50" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I50" s="7" t="inlineStr"/>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="H51" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I51" s="7" t="inlineStr"/>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="H52" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I52" s="7" t="inlineStr"/>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="H53" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I53" s="7" t="inlineStr"/>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="H54" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I54" s="7" t="inlineStr"/>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="H55" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I55" s="7" t="inlineStr"/>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="H56" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I56" s="7" t="inlineStr"/>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="H58" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I58" s="7" t="inlineStr"/>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="H59" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I59" s="7" t="inlineStr"/>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="H60" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I60" s="7" t="inlineStr"/>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="H61" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I61" s="7" t="inlineStr"/>
@@ -3620,7 +3620,7 @@
       </c>
       <c r="H62" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I62" s="7" t="inlineStr"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H63" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I63" s="7" t="inlineStr"/>
@@ -3722,7 +3722,7 @@
       </c>
       <c r="H64" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I64" s="7" t="inlineStr"/>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="H65" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I65" s="7" t="inlineStr"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="H66" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I66" s="7" t="inlineStr"/>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="H67" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I67" s="7" t="inlineStr"/>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="H68" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I68" s="7" t="inlineStr"/>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="H70" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I70" s="7" t="inlineStr"/>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="H71" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I71" s="7" t="inlineStr"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="H73" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I73" s="7" t="inlineStr"/>
@@ -4271,7 +4271,7 @@
       </c>
       <c r="H75" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I75" s="7" t="inlineStr"/>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="H76" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I76" s="7" t="inlineStr"/>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="H78" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I78" s="7" t="inlineStr"/>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H81" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I81" s="7" t="inlineStr"/>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="H83" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I83" s="7" t="inlineStr"/>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="H84" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I84" s="7" t="inlineStr"/>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="H85" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I85" s="7" t="inlineStr"/>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="H86" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I86" s="7" t="inlineStr"/>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="H87" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I87" s="7" t="inlineStr"/>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="H88" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I88" s="7" t="inlineStr"/>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="H90" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I90" s="7" t="inlineStr"/>
@@ -5118,7 +5118,7 @@
       </c>
       <c r="H92" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I92" s="7" t="inlineStr"/>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="H94" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I94" s="7" t="inlineStr"/>
@@ -5314,7 +5314,7 @@
       </c>
       <c r="H96" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I96" s="7" t="inlineStr"/>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="H104" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I104" s="7" t="inlineStr"/>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="H106" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I106" s="7" t="inlineStr"/>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="H108" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I108" s="7" t="inlineStr"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H110" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I110" s="7" t="inlineStr"/>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="H112" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I112" s="7" t="inlineStr"/>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="H114" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I114" s="7" t="inlineStr"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="H116" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I116" s="7" t="inlineStr"/>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="H118" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I118" s="7" t="inlineStr"/>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H121" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I121" s="7" t="inlineStr"/>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="H123" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I123" s="7" t="inlineStr"/>
@@ -6725,7 +6725,7 @@
       </c>
       <c r="H125" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I125" s="7" t="inlineStr"/>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="H128" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I128" s="7" t="inlineStr"/>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="H129" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I129" s="7" t="inlineStr"/>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="H131" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I131" s="7" t="inlineStr"/>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="H133" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I133" s="7" t="inlineStr"/>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="H134" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I134" s="7" t="inlineStr"/>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="H136" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I136" s="7" t="inlineStr"/>
@@ -7321,7 +7321,7 @@
       </c>
       <c r="H137" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I137" s="7" t="inlineStr"/>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="H139" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I139" s="7" t="inlineStr"/>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="H140" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I140" s="7" t="inlineStr"/>
@@ -7568,7 +7568,7 @@
       </c>
       <c r="H142" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I142" s="7" t="inlineStr"/>
@@ -7619,7 +7619,7 @@
       </c>
       <c r="H143" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I143" s="7" t="inlineStr"/>
@@ -7670,7 +7670,7 @@
       </c>
       <c r="H144" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I144" s="7" t="inlineStr"/>
@@ -7721,7 +7721,7 @@
       </c>
       <c r="H145" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I145" s="7" t="inlineStr"/>
@@ -7772,7 +7772,7 @@
       </c>
       <c r="H146" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I146" s="7" t="inlineStr"/>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="H147" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I147" s="7" t="inlineStr"/>
@@ -7874,7 +7874,7 @@
       </c>
       <c r="H148" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I148" s="7" t="inlineStr"/>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="H149" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I149" s="7" t="inlineStr"/>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="H150" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I150" s="7" t="inlineStr"/>
@@ -8027,7 +8027,7 @@
       </c>
       <c r="H151" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I151" s="7" t="inlineStr"/>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="H154" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I154" s="7" t="inlineStr"/>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="H155" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I155" s="7" t="inlineStr"/>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="H156" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I156" s="7" t="inlineStr"/>
@@ -8329,7 +8329,7 @@
       </c>
       <c r="H157" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I157" s="7" t="inlineStr"/>
@@ -8380,7 +8380,7 @@
       </c>
       <c r="H158" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I158" s="7" t="inlineStr"/>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="H159" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I159" s="7" t="inlineStr"/>
@@ -8482,7 +8482,7 @@
       </c>
       <c r="H160" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I160" s="7" t="inlineStr"/>
@@ -8533,7 +8533,7 @@
       </c>
       <c r="H161" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I161" s="7" t="inlineStr"/>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="H162" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I162" s="7" t="inlineStr"/>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="H163" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I163" s="7" t="inlineStr"/>
@@ -8686,7 +8686,7 @@
       </c>
       <c r="H164" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I164" s="7" t="inlineStr"/>
@@ -8737,7 +8737,7 @@
       </c>
       <c r="H165" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I165" s="7" t="inlineStr"/>
@@ -8788,7 +8788,7 @@
       </c>
       <c r="H166" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I166" s="7" t="inlineStr"/>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="H167" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I167" s="7" t="inlineStr"/>
@@ -8890,7 +8890,7 @@
       </c>
       <c r="H168" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I168" s="7" t="inlineStr"/>
@@ -8941,7 +8941,7 @@
       </c>
       <c r="H169" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I169" s="7" t="inlineStr"/>
@@ -8992,7 +8992,7 @@
       </c>
       <c r="H170" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I170" s="7" t="inlineStr"/>
@@ -9043,7 +9043,7 @@
       </c>
       <c r="H171" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I171" s="7" t="inlineStr"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="H172" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I172" s="7" t="inlineStr"/>
@@ -9145,7 +9145,7 @@
       </c>
       <c r="H173" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I173" s="7" t="inlineStr"/>
@@ -9196,7 +9196,7 @@
       </c>
       <c r="H174" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I174" s="7" t="inlineStr"/>
@@ -9298,7 +9298,7 @@
       </c>
       <c r="H176" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I176" s="7" t="inlineStr"/>
@@ -9396,7 +9396,7 @@
       </c>
       <c r="H178" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I178" s="7" t="inlineStr"/>
@@ -9447,7 +9447,7 @@
       </c>
       <c r="H179" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I179" s="7" t="inlineStr"/>
@@ -9498,7 +9498,7 @@
       </c>
       <c r="H180" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I180" s="7" t="inlineStr"/>
@@ -9549,7 +9549,7 @@
       </c>
       <c r="H181" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I181" s="7" t="inlineStr"/>
@@ -9600,7 +9600,7 @@
       </c>
       <c r="H182" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I182" s="7" t="inlineStr"/>
@@ -9651,7 +9651,7 @@
       </c>
       <c r="H183" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I183" s="7" t="inlineStr"/>
@@ -9753,7 +9753,7 @@
       </c>
       <c r="H185" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I185" s="7" t="inlineStr"/>
@@ -9804,7 +9804,7 @@
       </c>
       <c r="H186" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I186" s="7" t="inlineStr"/>
@@ -9855,7 +9855,7 @@
       </c>
       <c r="H187" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I187" s="7" t="inlineStr"/>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="H189" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I189" s="7" t="inlineStr"/>
@@ -10110,7 +10110,7 @@
       </c>
       <c r="H192" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I192" s="7" t="inlineStr"/>
@@ -10212,7 +10212,7 @@
       </c>
       <c r="H194" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I194" s="7" t="inlineStr"/>
@@ -10314,7 +10314,7 @@
       </c>
       <c r="H196" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I196" s="7" t="inlineStr"/>
@@ -10416,7 +10416,7 @@
       </c>
       <c r="H198" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I198" s="7" t="inlineStr"/>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="H201" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I201" s="7" t="inlineStr"/>
@@ -10667,7 +10667,7 @@
       </c>
       <c r="H203" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I203" s="7" t="inlineStr"/>
@@ -10769,7 +10769,7 @@
       </c>
       <c r="H205" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I205" s="7" t="inlineStr"/>
@@ -10871,7 +10871,7 @@
       </c>
       <c r="H207" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I207" s="7" t="inlineStr"/>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="H209" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I209" s="7" t="inlineStr"/>
@@ -11075,7 +11075,7 @@
       </c>
       <c r="H211" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I211" s="7" t="inlineStr"/>
@@ -11126,7 +11126,7 @@
       </c>
       <c r="H212" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I212" s="7" t="inlineStr"/>
@@ -11228,7 +11228,7 @@
       </c>
       <c r="H214" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I214" s="7" t="inlineStr"/>
@@ -11581,7 +11581,7 @@
       </c>
       <c r="H221" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I221" s="7" t="inlineStr"/>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="H230" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I230" s="7" t="inlineStr"/>
@@ -12142,7 +12142,7 @@
       </c>
       <c r="H232" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I232" s="7" t="inlineStr"/>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="H235" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I235" s="7" t="inlineStr"/>
@@ -12393,7 +12393,7 @@
       </c>
       <c r="H237" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I237" s="7" t="inlineStr"/>
@@ -12495,7 +12495,7 @@
       </c>
       <c r="H239" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I239" s="7" t="inlineStr"/>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="H241" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I241" s="7" t="inlineStr"/>
@@ -12648,7 +12648,7 @@
       </c>
       <c r="H242" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I242" s="7" t="inlineStr"/>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="H244" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I244" s="7" t="inlineStr"/>
@@ -12801,7 +12801,7 @@
       </c>
       <c r="H245" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I245" s="7" t="inlineStr"/>
@@ -12903,7 +12903,7 @@
       </c>
       <c r="H247" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I247" s="7" t="inlineStr"/>
@@ -12954,7 +12954,7 @@
       </c>
       <c r="H248" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I248" s="7" t="inlineStr"/>
@@ -13056,7 +13056,7 @@
       </c>
       <c r="H250" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I250" s="7" t="inlineStr"/>
@@ -13107,7 +13107,7 @@
       </c>
       <c r="H251" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I251" s="7" t="inlineStr"/>
@@ -13209,7 +13209,7 @@
       </c>
       <c r="H253" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I253" s="7" t="inlineStr"/>
@@ -13260,7 +13260,7 @@
       </c>
       <c r="H254" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I254" s="7" t="inlineStr"/>
@@ -13362,7 +13362,7 @@
       </c>
       <c r="H256" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I256" s="7" t="inlineStr"/>
@@ -13464,7 +13464,7 @@
       </c>
       <c r="H258" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I258" s="7" t="inlineStr"/>
@@ -13566,7 +13566,7 @@
       </c>
       <c r="H260" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I260" s="7" t="inlineStr"/>
@@ -13617,7 +13617,7 @@
       </c>
       <c r="H261" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I261" s="7" t="inlineStr"/>
@@ -13719,7 +13719,7 @@
       </c>
       <c r="H263" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I263" s="7" t="inlineStr"/>
@@ -13919,7 +13919,7 @@
       </c>
       <c r="H267" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I267" s="7" t="inlineStr"/>
@@ -13970,7 +13970,7 @@
       </c>
       <c r="H268" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I268" s="7" t="inlineStr"/>
@@ -14021,7 +14021,7 @@
       </c>
       <c r="H269" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I269" s="7" t="inlineStr"/>
@@ -14072,7 +14072,7 @@
       </c>
       <c r="H270" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I270" s="7" t="inlineStr"/>
@@ -14123,7 +14123,7 @@
       </c>
       <c r="H271" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250328</t>
         </is>
       </c>
       <c r="I271" s="7" t="inlineStr"/>
@@ -14378,7 +14378,7 @@
       </c>
       <c r="H276" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I276" s="7" t="inlineStr"/>
@@ -14429,7 +14429,7 @@
       </c>
       <c r="H277" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I277" s="7" t="inlineStr"/>
@@ -14480,7 +14480,7 @@
       </c>
       <c r="H278" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I278" s="7" t="inlineStr"/>
@@ -14531,7 +14531,7 @@
       </c>
       <c r="H279" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250228</t>
         </is>
       </c>
       <c r="I279" s="7" t="inlineStr"/>
@@ -15092,7 +15092,7 @@
       </c>
       <c r="H290" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I290" s="7" t="inlineStr"/>
@@ -15143,7 +15143,7 @@
       </c>
       <c r="H291" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I291" s="7" t="inlineStr"/>
@@ -15296,7 +15296,7 @@
       </c>
       <c r="H294" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I294" s="7" t="inlineStr"/>
@@ -15398,7 +15398,7 @@
       </c>
       <c r="H296" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I296" s="7" t="inlineStr"/>
@@ -15449,7 +15449,7 @@
       </c>
       <c r="H297" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I297" s="7" t="inlineStr"/>
@@ -15551,7 +15551,7 @@
       </c>
       <c r="H299" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I299" s="7" t="inlineStr"/>
@@ -15602,7 +15602,7 @@
       </c>
       <c r="H300" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I300" s="7" t="inlineStr"/>
@@ -15653,7 +15653,7 @@
       </c>
       <c r="H301" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I301" s="7" t="inlineStr"/>
@@ -15704,7 +15704,7 @@
       </c>
       <c r="H302" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I302" s="7" t="inlineStr"/>
@@ -15755,7 +15755,7 @@
       </c>
       <c r="H303" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I303" s="7" t="inlineStr"/>
@@ -15806,7 +15806,7 @@
       </c>
       <c r="H304" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I304" s="7" t="inlineStr"/>
@@ -15857,7 +15857,7 @@
       </c>
       <c r="H305" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I305" s="7" t="inlineStr"/>
@@ -15908,7 +15908,7 @@
       </c>
       <c r="H306" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I306" s="7" t="inlineStr"/>
@@ -15959,7 +15959,7 @@
       </c>
       <c r="H307" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I307" s="7" t="inlineStr"/>
@@ -16010,7 +16010,7 @@
       </c>
       <c r="H308" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I308" s="7" t="inlineStr"/>
@@ -16061,7 +16061,7 @@
       </c>
       <c r="H309" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I309" s="7" t="inlineStr"/>
@@ -16112,7 +16112,7 @@
       </c>
       <c r="H310" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250514</t>
         </is>
       </c>
       <c r="I310" s="7" t="inlineStr"/>
@@ -17009,7 +17009,7 @@
       </c>
       <c r="H329" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I329" s="7" t="inlineStr"/>
@@ -17060,7 +17060,7 @@
       </c>
       <c r="H330" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I330" s="7" t="inlineStr"/>
@@ -17111,7 +17111,7 @@
       </c>
       <c r="H331" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I331" s="7" t="inlineStr"/>
@@ -17162,7 +17162,7 @@
       </c>
       <c r="H332" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I332" s="7" t="inlineStr"/>
@@ -17213,7 +17213,7 @@
       </c>
       <c r="H333" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I333" s="7" t="inlineStr"/>
@@ -17264,7 +17264,7 @@
       </c>
       <c r="H334" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I334" s="7" t="inlineStr"/>
@@ -17315,7 +17315,7 @@
       </c>
       <c r="H335" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I335" s="7" t="inlineStr"/>
@@ -17366,7 +17366,7 @@
       </c>
       <c r="H336" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I336" s="7" t="inlineStr"/>
@@ -17417,7 +17417,7 @@
       </c>
       <c r="H337" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I337" s="7" t="inlineStr"/>
@@ -17468,7 +17468,7 @@
       </c>
       <c r="H338" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I338" s="7" t="inlineStr"/>
@@ -17519,7 +17519,7 @@
       </c>
       <c r="H339" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I339" s="7" t="inlineStr"/>
@@ -17570,7 +17570,7 @@
       </c>
       <c r="H340" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I340" s="7" t="inlineStr"/>
@@ -17621,7 +17621,7 @@
       </c>
       <c r="H341" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I341" s="7" t="inlineStr"/>
@@ -17672,7 +17672,7 @@
       </c>
       <c r="H342" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I342" s="7" t="inlineStr"/>
@@ -17723,7 +17723,7 @@
       </c>
       <c r="H343" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I343" s="7" t="inlineStr"/>
@@ -17774,7 +17774,7 @@
       </c>
       <c r="H344" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I344" s="7" t="inlineStr"/>
@@ -17825,7 +17825,7 @@
       </c>
       <c r="H345" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I345" s="7" t="inlineStr"/>
@@ -17876,7 +17876,7 @@
       </c>
       <c r="H346" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I346" s="7" t="inlineStr"/>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="H347" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I347" s="7" t="inlineStr"/>
@@ -17978,7 +17978,7 @@
       </c>
       <c r="H348" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I348" s="7" t="inlineStr"/>
@@ -18029,7 +18029,7 @@
       </c>
       <c r="H349" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I349" s="7" t="inlineStr"/>
@@ -18080,7 +18080,7 @@
       </c>
       <c r="H350" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I350" s="7" t="inlineStr"/>
@@ -18131,7 +18131,7 @@
       </c>
       <c r="H351" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I351" s="7" t="inlineStr"/>
@@ -18182,7 +18182,7 @@
       </c>
       <c r="H352" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I352" s="7" t="inlineStr"/>
@@ -18233,7 +18233,7 @@
       </c>
       <c r="H353" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I353" s="7" t="inlineStr"/>
@@ -18284,7 +18284,7 @@
       </c>
       <c r="H354" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I354" s="7" t="inlineStr"/>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="H355" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I355" s="7" t="inlineStr"/>
@@ -18386,7 +18386,7 @@
       </c>
       <c r="H356" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I356" s="7" t="inlineStr"/>
@@ -18437,7 +18437,7 @@
       </c>
       <c r="H357" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I357" s="7" t="inlineStr"/>
@@ -18488,7 +18488,7 @@
       </c>
       <c r="H358" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I358" s="7" t="inlineStr"/>
@@ -18539,7 +18539,7 @@
       </c>
       <c r="H359" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I359" s="7" t="inlineStr"/>
@@ -18590,7 +18590,7 @@
       </c>
       <c r="H360" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I360" s="7" t="inlineStr"/>
@@ -18641,7 +18641,7 @@
       </c>
       <c r="H361" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I361" s="7" t="inlineStr"/>
@@ -18692,7 +18692,7 @@
       </c>
       <c r="H362" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I362" s="7" t="inlineStr"/>
@@ -18743,7 +18743,7 @@
       </c>
       <c r="H363" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250612</t>
         </is>
       </c>
       <c r="I363" s="7" t="inlineStr"/>
@@ -18794,7 +18794,7 @@
       </c>
       <c r="H364" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I364" s="7" t="inlineStr"/>
@@ -18845,7 +18845,7 @@
       </c>
       <c r="H365" s="7" t="inlineStr">
         <is>
-          <t>20250702</t>
+          <t>20250428</t>
         </is>
       </c>
       <c r="I365" s="7" t="inlineStr"/>

</xml_diff>